<commit_message>
Group Final commit #6 gameList.csv updated
</commit_message>
<xml_diff>
--- a/src/Databases/gameList.xlsx
+++ b/src/Databases/gameList.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df73c3b01a98b0e2/Documents/Sheridan College/Object Oriented Programming 2/GameInventoryManager/src/Databases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heckd\OneDrive\Documents\Sheridan College\Object Oriented Programming 2\GameInventoryManager\src\Databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{098D4AC8-708F-4C84-BD09-FB6D884AAFA1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{CBAE4755-8AF3-4A8E-9408-3D6B86D107B2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{AD280204-4D64-41C1-B860-09F2BD143020}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4178" yWindow="2033" windowWidth="21599" windowHeight="11872" xr2:uid="{D2B05FC2-3B9B-40D7-AE79-F6AB6DED50AD}"/>
+    <workbookView xWindow="2663" yWindow="2085" windowWidth="16604" windowHeight="12420" xr2:uid="{D2B05FC2-3B9B-40D7-AE79-F6AB6DED50AD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="gameList.xml" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="102">
   <si>
     <t>Game Title</t>
   </si>
@@ -67,19 +67,295 @@
   </si>
   <si>
     <t>Franchise</t>
+  </si>
+  <si>
+    <t>Borderlands 2</t>
+  </si>
+  <si>
+    <t>Payday 2</t>
+  </si>
+  <si>
+    <t>Destiny 2</t>
+  </si>
+  <si>
+    <t>CSGO</t>
+  </si>
+  <si>
+    <t>Dota 2</t>
+  </si>
+  <si>
+    <t>Fortnite</t>
+  </si>
+  <si>
+    <t>Tetris</t>
+  </si>
+  <si>
+    <t>Garrys Mod</t>
+  </si>
+  <si>
+    <t>Overwatch</t>
+  </si>
+  <si>
+    <t>World of Warcraft</t>
+  </si>
+  <si>
+    <t>Rim World</t>
+  </si>
+  <si>
+    <t>Astroneer</t>
+  </si>
+  <si>
+    <t>Shellshock</t>
+  </si>
+  <si>
+    <t>Spintires</t>
+  </si>
+  <si>
+    <t>Cities: Skylines</t>
+  </si>
+  <si>
+    <t>HELLDIVERS</t>
+  </si>
+  <si>
+    <t>Stick Fight</t>
+  </si>
+  <si>
+    <t>DOOM</t>
+  </si>
+  <si>
+    <t>SIX SIEGE</t>
+  </si>
+  <si>
+    <t>Verdun</t>
+  </si>
+  <si>
+    <t>The Witcher 3</t>
+  </si>
+  <si>
+    <t>Stellaris</t>
+  </si>
+  <si>
+    <t>Rocket League</t>
+  </si>
+  <si>
+    <t>Battlerite</t>
+  </si>
+  <si>
+    <t>GTA V</t>
+  </si>
+  <si>
+    <t>Gang Beasts</t>
+  </si>
+  <si>
+    <t>Golf With Your Friends</t>
+  </si>
+  <si>
+    <t>Move or Die</t>
+  </si>
+  <si>
+    <t>Windward</t>
+  </si>
+  <si>
+    <t>ABZU</t>
+  </si>
+  <si>
+    <t>Blackwake</t>
+  </si>
+  <si>
+    <t>Dishonored</t>
+  </si>
+  <si>
+    <t>Elite Dangerous</t>
+  </si>
+  <si>
+    <t>Far Cry 3</t>
+  </si>
+  <si>
+    <t>Hitman Absolution</t>
+  </si>
+  <si>
+    <t>Tower Unite</t>
+  </si>
+  <si>
+    <t>Killing Floor 2</t>
+  </si>
+  <si>
+    <t>Mad Max</t>
+  </si>
+  <si>
+    <t>Tomb Raider</t>
+  </si>
+  <si>
+    <t>Watch_Dogs</t>
+  </si>
+  <si>
+    <t>Bully: Scholarship edition</t>
+  </si>
+  <si>
+    <t>Wolfenstein</t>
+  </si>
+  <si>
+    <t>Alien: Isolation</t>
+  </si>
+  <si>
+    <t>Subnautica</t>
+  </si>
+  <si>
+    <t>Total War: WARHAMMER</t>
+  </si>
+  <si>
+    <t>The Ship: Remastered</t>
+  </si>
+  <si>
+    <t>MSGV</t>
+  </si>
+  <si>
+    <t>Poly Bridge</t>
+  </si>
+  <si>
+    <t>Slime Rancher</t>
+  </si>
+  <si>
+    <t>Spore</t>
+  </si>
+  <si>
+    <t>Stardew Valley</t>
+  </si>
+  <si>
+    <t>Shoppe Keep</t>
+  </si>
+  <si>
+    <t>Tropico 4</t>
+  </si>
+  <si>
+    <t>Space Engineer</t>
+  </si>
+  <si>
+    <t>Project Highrise</t>
+  </si>
+  <si>
+    <t>Cobalt</t>
+  </si>
+  <si>
+    <t>Crawl</t>
+  </si>
+  <si>
+    <t>More of Die</t>
+  </si>
+  <si>
+    <t>Miner Meltdown</t>
+  </si>
+  <si>
+    <t>Tabletop Simulator</t>
+  </si>
+  <si>
+    <t>XCOM: Enemy Unknown</t>
+  </si>
+  <si>
+    <t>Poker Night 2</t>
+  </si>
+  <si>
+    <t>Mass Effect 2</t>
+  </si>
+  <si>
+    <t>Bioshock Infinite</t>
+  </si>
+  <si>
+    <t>Sonic Adventure 2</t>
+  </si>
+  <si>
+    <t>Counter Strike Source</t>
+  </si>
+  <si>
+    <t>Unturned</t>
+  </si>
+  <si>
+    <t>Prison Architect</t>
+  </si>
+  <si>
+    <t>The Ultimate Vault Hunter’s Upgrade lets you get the most out of the Borderlands 2 experience.</t>
+  </si>
+  <si>
+    <t>Aspyr</t>
+  </si>
+  <si>
+    <t>Gearbox Software</t>
+  </si>
+  <si>
+    <t>69/75</t>
+  </si>
+  <si>
+    <t>FPS</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>PAYDAY 2 is an action-packed, four-player co-op shooter that once again lets gamers don the masks of the original PAYDAY crew</t>
+  </si>
+  <si>
+    <t>Starbreeze</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>OVERKILL</t>
+  </si>
+  <si>
+    <t>526/1130</t>
+  </si>
+  <si>
+    <t>PAYDAY</t>
+  </si>
+  <si>
+    <t>Borderlands</t>
+  </si>
+  <si>
+    <t>Destiny</t>
+  </si>
+  <si>
+    <t>Destiny 2 is an online-only multiplayer first-person shooter video game developed by Bungie. It was released for PlayStation 4 and Xbox One on September 6, 2017, followed by a Microsoft Windows version the following month</t>
+  </si>
+  <si>
+    <t>Bungie</t>
+  </si>
+  <si>
+    <t>432/945</t>
+  </si>
+  <si>
+    <t>Counter-Strike: Global Offensive is a multiplayer first-person shooter video game developed by Hidden Path Entertainment and Valve Corporation.</t>
+  </si>
+  <si>
+    <t>Valve</t>
+  </si>
+  <si>
+    <t>167/167</t>
+  </si>
+  <si>
+    <t>Counter Strike</t>
+  </si>
+  <si>
+    <t>Every day, millions of players worldwide enter battle as one of over a hundred Dota heroes. And no matter if it's their 10th hour of play or 1,000th, there's always something new to discover. With regular updates that ensure a constant evolution of gameplay, features, and heroes, Dota 2 has taken on a life of its own.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,8 +378,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,16 +695,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B572673-7001-44C9-92F2-2F317210CB5B}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:L69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.86328125" customWidth="1"/>
-    <col min="2" max="2" width="10.53125" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="36.46484375" customWidth="1"/>
     <col min="3" max="3" width="6.33203125" customWidth="1"/>
     <col min="5" max="5" width="12.19921875" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" customWidth="1"/>
@@ -435,7 +712,7 @@
     <col min="12" max="12" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,13 +747,492 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2">
+        <v>21.99</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2">
+        <v>2012</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2">
+        <v>89</v>
+      </c>
+      <c r="I2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3">
+        <v>11.49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3">
+        <v>2013</v>
+      </c>
+      <c r="F3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3">
+        <v>79</v>
+      </c>
+      <c r="I3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="D4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4">
+        <v>2013</v>
+      </c>
+      <c r="F4">
+        <v>80</v>
+      </c>
+      <c r="G4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4">
+        <v>87</v>
+      </c>
+      <c r="I4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5">
+        <v>4.99</v>
+      </c>
+      <c r="D5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5">
+        <v>2012</v>
+      </c>
+      <c r="F5">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5">
+        <v>94</v>
+      </c>
+      <c r="I5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" t="s">
+        <v>85</v>
+      </c>
+      <c r="L5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Group Final commit #7 I've added a lot of stuff for database interaction It's pretty much taking it all in. Need second scene, 2 more data bases, display data correctly, intreaction likt edit, remove, add still needed
</commit_message>
<xml_diff>
--- a/src/Databases/gameList.xlsx
+++ b/src/Databases/gameList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heckd\OneDrive\Documents\Sheridan College\Object Oriented Programming 2\GameInventoryManager\src\Databases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df73c3b01a98b0e2/Documents/Sheridan College/Object Oriented Programming 2/GameInventoryManager/src/Databases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{CBAE4755-8AF3-4A8E-9408-3D6B86D107B2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{AD280204-4D64-41C1-B860-09F2BD143020}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="8_{CBAE4755-8AF3-4A8E-9408-3D6B86D107B2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{FB0042AF-45F4-4FD8-A604-0A2FE871B081}"/>
   <bookViews>
-    <workbookView xWindow="2663" yWindow="2085" windowWidth="16604" windowHeight="12420" xr2:uid="{D2B05FC2-3B9B-40D7-AE79-F6AB6DED50AD}"/>
+    <workbookView xWindow="-487" yWindow="1267" windowWidth="16604" windowHeight="12420" xr2:uid="{D2B05FC2-3B9B-40D7-AE79-F6AB6DED50AD}"/>
   </bookViews>
   <sheets>
     <sheet name="gameList.xml" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="131">
   <si>
     <t>Game Title</t>
   </si>
@@ -297,9 +297,6 @@
     <t>Starbreeze</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>OVERKILL</t>
   </si>
   <si>
@@ -337,13 +334,103 @@
   </si>
   <si>
     <t>Every day, millions of players worldwide enter battle as one of over a hundred Dota heroes. And no matter if it's their 10th hour of play or 1,000th, there's always something new to discover. With regular updates that ensure a constant evolution of gameplay, features, and heroes, Dota 2 has taken on a life of its own.</t>
+  </si>
+  <si>
+    <t>Fortnite is an online video game developed by Epic Games and released in 2017. It is available in three distinct game mode versions that otherwise share the same general gameplay</t>
+  </si>
+  <si>
+    <t>Epic Games</t>
+  </si>
+  <si>
+    <t>Epic games</t>
+  </si>
+  <si>
+    <t>0/540</t>
+  </si>
+  <si>
+    <t>0/983</t>
+  </si>
+  <si>
+    <t>MMRPG</t>
+  </si>
+  <si>
+    <t>Dota</t>
+  </si>
+  <si>
+    <t>Tetris is a tile-matching puzzle video game originally designed and programmed by Soviet Russian game designer Alexey Leonidovich Pajitnov. The first playable version was completed on June 6, 1984, while he was working for the Dorodnitsyn Computing Centre of the Academy of Science of the Soviet Union in Moscow.</t>
+  </si>
+  <si>
+    <t>Alexey Pajitnov</t>
+  </si>
+  <si>
+    <t>Sega</t>
+  </si>
+  <si>
+    <t>0/30</t>
+  </si>
+  <si>
+    <t>Arcade</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Garry's Mod is a physics sandbox. There aren't any predefined aims or goals. We give you the tools and leave you to play.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facepunch </t>
+  </si>
+  <si>
+    <t>0/10</t>
+  </si>
+  <si>
+    <t>Sandbox</t>
+  </si>
+  <si>
+    <t>Garry's Mod</t>
+  </si>
+  <si>
+    <t>Overwatch is a team-based multiplayer first-person shooter developed and published by Blizzard Entertainment and released on May 24, 2016, for PlayStation 4, Xbox One, and Windows.</t>
+  </si>
+  <si>
+    <t>0/140</t>
+  </si>
+  <si>
+    <t>World of Warcraft is a massively multiplayer online role-playing game released in 2004 by Blizzard Entertainment. It is the fourth released game set in the Warcraft fantasy universe</t>
+  </si>
+  <si>
+    <t>130/800</t>
+  </si>
+  <si>
+    <t>RPG</t>
+  </si>
+  <si>
+    <t>WoW</t>
+  </si>
+  <si>
+    <t>A sci-fi colony sim driven by an intelligent AI storyteller. Inspired by Dwarf Fortress and Firefly. Generates stories by simulating psychology, ecology, gunplay, melee combat, climate, biomes, diplomacy, interpersonal relationships, art, medicine, trade, and more.</t>
+  </si>
+  <si>
+    <t>Ludeon Studiers</t>
+  </si>
+  <si>
+    <t>Ludeon Studies</t>
+  </si>
+  <si>
+    <t>44/70</t>
+  </si>
+  <si>
+    <t>Surivial</t>
+  </si>
+  <si>
+    <t>RimWorld</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,6 +440,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="6"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -378,9 +472,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B572673-7001-44C9-92F2-2F317210CB5B}">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -785,7 +880,7 @@
         <v>85</v>
       </c>
       <c r="L2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
@@ -804,17 +899,17 @@
       <c r="E3">
         <v>2013</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>88</v>
-      </c>
-      <c r="G3" t="s">
-        <v>89</v>
       </c>
       <c r="H3">
         <v>79</v>
       </c>
       <c r="I3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J3" t="s">
         <v>84</v>
@@ -823,7 +918,7 @@
         <v>85</v>
       </c>
       <c r="L3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
@@ -831,13 +926,13 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4">
         <v>19.989999999999998</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E4">
         <v>2013</v>
@@ -846,13 +941,13 @@
         <v>80</v>
       </c>
       <c r="G4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H4">
         <v>87</v>
       </c>
       <c r="I4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J4" t="s">
         <v>84</v>
@@ -861,7 +956,7 @@
         <v>85</v>
       </c>
       <c r="L4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.4" x14ac:dyDescent="0.45">
@@ -869,13 +964,13 @@
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C5">
         <v>4.99</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E5">
         <v>2012</v>
@@ -884,13 +979,13 @@
         <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H5">
         <v>94</v>
       </c>
       <c r="I5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J5" t="s">
         <v>84</v>
@@ -899,7 +994,7 @@
         <v>85</v>
       </c>
       <c r="L5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.4" x14ac:dyDescent="0.45">
@@ -907,43 +1002,265 @@
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="E6">
+        <v>2013</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6">
+        <v>85</v>
+      </c>
+      <c r="I6" t="s">
+        <v>105</v>
+      </c>
+      <c r="J6" t="s">
+        <v>106</v>
+      </c>
+      <c r="K6" t="s">
+        <v>85</v>
+      </c>
+      <c r="L6" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>17</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7">
+        <v>2017</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7">
+        <v>40</v>
+      </c>
+      <c r="I7" t="s">
+        <v>104</v>
+      </c>
+      <c r="J7" t="s">
+        <v>84</v>
+      </c>
+      <c r="K7" t="s">
+        <v>85</v>
+      </c>
+      <c r="L7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>18</v>
       </c>
+      <c r="B8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8">
+        <v>4.99</v>
+      </c>
+      <c r="D8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8">
+        <v>1984</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H8">
+        <v>93</v>
+      </c>
+      <c r="I8" t="s">
+        <v>111</v>
+      </c>
+      <c r="J8" t="s">
+        <v>112</v>
+      </c>
+      <c r="K8" t="s">
+        <v>113</v>
+      </c>
+      <c r="L8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9">
+        <v>10.99</v>
+      </c>
+      <c r="D9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9">
+        <v>2006</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>115</v>
+      </c>
+      <c r="H9">
+        <v>100</v>
+      </c>
+      <c r="I9" t="s">
+        <v>116</v>
+      </c>
+      <c r="J9" t="s">
+        <v>117</v>
+      </c>
+      <c r="K9" t="s">
+        <v>85</v>
+      </c>
+      <c r="L9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10">
+        <v>59.99</v>
+      </c>
+      <c r="D10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10">
+        <v>2015</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10">
+        <v>93</v>
+      </c>
+      <c r="I10" t="s">
+        <v>120</v>
+      </c>
+      <c r="J10" t="s">
+        <v>84</v>
+      </c>
+      <c r="K10" t="s">
+        <v>85</v>
+      </c>
+      <c r="L10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="D11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11">
+        <v>2004</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11">
+        <v>88</v>
+      </c>
+      <c r="I11" t="s">
+        <v>122</v>
+      </c>
+      <c r="J11" t="s">
+        <v>123</v>
+      </c>
+      <c r="K11" t="s">
+        <v>85</v>
+      </c>
+      <c r="L11" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12">
+        <v>39.99</v>
+      </c>
+      <c r="D12" t="s">
+        <v>126</v>
+      </c>
+      <c r="E12">
+        <v>2018</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>127</v>
+      </c>
+      <c r="H12">
+        <v>86</v>
+      </c>
+      <c r="I12" t="s">
+        <v>128</v>
+      </c>
+      <c r="J12" t="s">
+        <v>129</v>
+      </c>
+      <c r="K12" t="s">
+        <v>113</v>
+      </c>
+      <c r="L12" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">

</xml_diff>